<commit_message>
cleaned up the semdis novelty corrs excel sheet
</commit_message>
<xml_diff>
--- a/results/novelty_algos_semdis_corrs_results_070821.xlsx
+++ b/results/novelty_algos_semdis_corrs_results_070821.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhec8\Documents\Northwestern_SROP\AUT-Scoring\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7190BFC-37C3-48FB-A6AF-2F2CA3022BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1D8327-F1BC-4A1F-BCBC-552CF8DECFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2415" yWindow="2010" windowWidth="21495" windowHeight="11490" xr2:uid="{764781FE-4BAD-447C-A1C0-C9E30184FB66}"/>
   </bookViews>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -174,11 +174,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -488,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C86FAE-829A-4700-A264-DD1DD0D29EE6}">
-  <dimension ref="A1:C285"/>
+  <dimension ref="A1:C817"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="48" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>6</v>
       </c>
@@ -2122,7 +2154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>3</v>
       </c>
@@ -2964,7 +2996,1613 @@
         <v>1.4500000000000001E-2</v>
       </c>
     </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C286" s="7"/>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C287" s="7"/>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C288" s="7"/>
+    </row>
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C289" s="7"/>
+    </row>
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C290" s="7"/>
+    </row>
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C291" s="7"/>
+    </row>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C292" s="7"/>
+    </row>
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C293" s="7"/>
+    </row>
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C294" s="7"/>
+    </row>
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C295" s="7"/>
+    </row>
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C296" s="7"/>
+    </row>
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C297" s="7"/>
+    </row>
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C298" s="7"/>
+    </row>
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C299" s="7"/>
+    </row>
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C300" s="7"/>
+    </row>
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C301" s="7"/>
+    </row>
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C302" s="7"/>
+    </row>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C303" s="7"/>
+    </row>
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C304" s="7"/>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C305" s="7"/>
+    </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C306" s="7"/>
+    </row>
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C307" s="7"/>
+    </row>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C308" s="7"/>
+    </row>
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C309" s="7"/>
+    </row>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C310" s="7"/>
+    </row>
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C311" s="7"/>
+    </row>
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C312" s="7"/>
+    </row>
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C313" s="7"/>
+    </row>
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C314" s="7"/>
+    </row>
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C315" s="7"/>
+    </row>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C316" s="7"/>
+    </row>
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C317" s="7"/>
+    </row>
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C318" s="7"/>
+    </row>
+    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C319" s="7"/>
+    </row>
+    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C320" s="7"/>
+    </row>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C321" s="7"/>
+    </row>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C322" s="7"/>
+    </row>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C323" s="7"/>
+    </row>
+    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C324" s="7"/>
+    </row>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C325" s="7"/>
+    </row>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C326" s="7"/>
+    </row>
+    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C327" s="7"/>
+    </row>
+    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C328" s="7"/>
+    </row>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C329" s="7"/>
+    </row>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C330" s="7"/>
+    </row>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C331" s="7"/>
+    </row>
+    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C332" s="7"/>
+    </row>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C333" s="7"/>
+    </row>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C334" s="7"/>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C335" s="7"/>
+    </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C336" s="7"/>
+    </row>
+    <row r="337" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C337" s="7"/>
+    </row>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C338" s="7"/>
+    </row>
+    <row r="339" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C339" s="7"/>
+    </row>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C340" s="7"/>
+    </row>
+    <row r="341" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C341" s="7"/>
+    </row>
+    <row r="342" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C342" s="7"/>
+    </row>
+    <row r="343" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C343" s="7"/>
+    </row>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C344" s="7"/>
+    </row>
+    <row r="345" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C345" s="7"/>
+    </row>
+    <row r="346" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C346" s="7"/>
+    </row>
+    <row r="347" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C347" s="7"/>
+    </row>
+    <row r="348" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C348" s="7"/>
+    </row>
+    <row r="349" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C349" s="7"/>
+    </row>
+    <row r="350" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C350" s="7"/>
+    </row>
+    <row r="351" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C351" s="7"/>
+    </row>
+    <row r="352" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C352" s="7"/>
+    </row>
+    <row r="353" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C353" s="7"/>
+    </row>
+    <row r="354" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C354" s="7"/>
+    </row>
+    <row r="355" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C355" s="7"/>
+    </row>
+    <row r="356" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C356" s="7"/>
+    </row>
+    <row r="357" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C357" s="7"/>
+    </row>
+    <row r="358" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C358" s="7"/>
+    </row>
+    <row r="359" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C359" s="7"/>
+    </row>
+    <row r="360" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C360" s="7"/>
+    </row>
+    <row r="361" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C361" s="7"/>
+    </row>
+    <row r="362" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C362" s="7"/>
+    </row>
+    <row r="363" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C363" s="7"/>
+    </row>
+    <row r="364" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C364" s="7"/>
+    </row>
+    <row r="365" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C365" s="7"/>
+    </row>
+    <row r="366" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C366" s="7"/>
+    </row>
+    <row r="367" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C367" s="7"/>
+    </row>
+    <row r="368" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C368" s="7"/>
+    </row>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C369" s="7"/>
+    </row>
+    <row r="370" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C370" s="7"/>
+    </row>
+    <row r="371" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C371" s="7"/>
+    </row>
+    <row r="372" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C372" s="7"/>
+    </row>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C373" s="7"/>
+    </row>
+    <row r="374" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C374" s="7"/>
+    </row>
+    <row r="375" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C375" s="7"/>
+    </row>
+    <row r="376" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C376" s="7"/>
+    </row>
+    <row r="377" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C377" s="7"/>
+    </row>
+    <row r="378" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C378" s="7"/>
+    </row>
+    <row r="379" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C379" s="7"/>
+    </row>
+    <row r="380" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C380" s="7"/>
+    </row>
+    <row r="381" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C381" s="7"/>
+    </row>
+    <row r="382" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C382" s="7"/>
+    </row>
+    <row r="383" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C383" s="7"/>
+    </row>
+    <row r="384" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C384" s="7"/>
+    </row>
+    <row r="385" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C385" s="7"/>
+    </row>
+    <row r="386" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C386" s="7"/>
+    </row>
+    <row r="387" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C387" s="7"/>
+    </row>
+    <row r="388" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C388" s="7"/>
+    </row>
+    <row r="389" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C389" s="7"/>
+    </row>
+    <row r="390" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C390" s="7"/>
+    </row>
+    <row r="391" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C391" s="7"/>
+    </row>
+    <row r="392" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C392" s="7"/>
+    </row>
+    <row r="393" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C393" s="7"/>
+    </row>
+    <row r="394" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C394" s="7"/>
+    </row>
+    <row r="395" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C395" s="7"/>
+    </row>
+    <row r="396" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C396" s="7"/>
+    </row>
+    <row r="397" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C397" s="7"/>
+    </row>
+    <row r="398" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C398" s="7"/>
+    </row>
+    <row r="399" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C399" s="7"/>
+    </row>
+    <row r="400" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C400" s="7"/>
+    </row>
+    <row r="401" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C401" s="7"/>
+    </row>
+    <row r="402" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C402" s="7"/>
+    </row>
+    <row r="403" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C403" s="7"/>
+    </row>
+    <row r="404" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C404" s="7"/>
+    </row>
+    <row r="405" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C405" s="7"/>
+    </row>
+    <row r="406" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C406" s="7"/>
+    </row>
+    <row r="407" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C407" s="7"/>
+    </row>
+    <row r="408" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C408" s="7"/>
+    </row>
+    <row r="409" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C409" s="7"/>
+    </row>
+    <row r="410" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C410" s="7"/>
+    </row>
+    <row r="411" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C411" s="7"/>
+    </row>
+    <row r="412" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C412" s="7"/>
+    </row>
+    <row r="413" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C413" s="7"/>
+    </row>
+    <row r="414" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C414" s="7"/>
+    </row>
+    <row r="415" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C415" s="7"/>
+    </row>
+    <row r="416" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C416" s="7"/>
+    </row>
+    <row r="417" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C417" s="7"/>
+    </row>
+    <row r="418" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C418" s="7"/>
+    </row>
+    <row r="419" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C419" s="7"/>
+    </row>
+    <row r="420" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C420" s="7"/>
+    </row>
+    <row r="421" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C421" s="7"/>
+    </row>
+    <row r="422" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C422" s="7"/>
+    </row>
+    <row r="423" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C423" s="7"/>
+    </row>
+    <row r="424" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C424" s="7"/>
+    </row>
+    <row r="425" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C425" s="7"/>
+    </row>
+    <row r="426" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C426" s="7"/>
+    </row>
+    <row r="427" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C427" s="7"/>
+    </row>
+    <row r="428" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C428" s="7"/>
+    </row>
+    <row r="429" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C429" s="7"/>
+    </row>
+    <row r="430" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C430" s="7"/>
+    </row>
+    <row r="431" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C431" s="7"/>
+    </row>
+    <row r="432" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C432" s="7"/>
+    </row>
+    <row r="433" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C433" s="7"/>
+    </row>
+    <row r="434" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C434" s="7"/>
+    </row>
+    <row r="435" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C435" s="7"/>
+    </row>
+    <row r="436" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C436" s="7"/>
+    </row>
+    <row r="437" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C437" s="7"/>
+    </row>
+    <row r="438" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C438" s="7"/>
+    </row>
+    <row r="439" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C439" s="7"/>
+    </row>
+    <row r="440" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C440" s="7"/>
+    </row>
+    <row r="441" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C441" s="7"/>
+    </row>
+    <row r="442" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C442" s="7"/>
+    </row>
+    <row r="443" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C443" s="7"/>
+    </row>
+    <row r="444" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C444" s="7"/>
+    </row>
+    <row r="445" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C445" s="7"/>
+    </row>
+    <row r="446" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C446" s="7"/>
+    </row>
+    <row r="447" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C447" s="7"/>
+    </row>
+    <row r="448" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C448" s="7"/>
+    </row>
+    <row r="449" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C449" s="7"/>
+    </row>
+    <row r="450" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C450" s="7"/>
+    </row>
+    <row r="451" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C451" s="7"/>
+    </row>
+    <row r="452" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C452" s="7"/>
+    </row>
+    <row r="453" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C453" s="7"/>
+    </row>
+    <row r="454" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C454" s="7"/>
+    </row>
+    <row r="455" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C455" s="7"/>
+    </row>
+    <row r="456" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C456" s="7"/>
+    </row>
+    <row r="457" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C457" s="7"/>
+    </row>
+    <row r="458" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C458" s="7"/>
+    </row>
+    <row r="459" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C459" s="7"/>
+    </row>
+    <row r="460" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C460" s="7"/>
+    </row>
+    <row r="461" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C461" s="7"/>
+    </row>
+    <row r="462" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C462" s="7"/>
+    </row>
+    <row r="463" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C463" s="7"/>
+    </row>
+    <row r="464" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C464" s="7"/>
+    </row>
+    <row r="465" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C465" s="7"/>
+    </row>
+    <row r="466" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C466" s="7"/>
+    </row>
+    <row r="467" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C467" s="7"/>
+    </row>
+    <row r="468" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C468" s="7"/>
+    </row>
+    <row r="469" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C469" s="7"/>
+    </row>
+    <row r="470" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C470" s="7"/>
+    </row>
+    <row r="471" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C471" s="7"/>
+    </row>
+    <row r="472" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C472" s="7"/>
+    </row>
+    <row r="473" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C473" s="7"/>
+    </row>
+    <row r="474" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C474" s="7"/>
+    </row>
+    <row r="475" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C475" s="7"/>
+    </row>
+    <row r="476" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C476" s="7"/>
+    </row>
+    <row r="477" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C477" s="7"/>
+    </row>
+    <row r="478" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C478" s="7"/>
+    </row>
+    <row r="479" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C479" s="7"/>
+    </row>
+    <row r="480" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C480" s="7"/>
+    </row>
+    <row r="481" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C481" s="7"/>
+    </row>
+    <row r="482" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C482" s="7"/>
+    </row>
+    <row r="483" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C483" s="7"/>
+    </row>
+    <row r="484" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C484" s="7"/>
+    </row>
+    <row r="485" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C485" s="7"/>
+    </row>
+    <row r="486" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C486" s="7"/>
+    </row>
+    <row r="487" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C487" s="7"/>
+    </row>
+    <row r="488" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C488" s="7"/>
+    </row>
+    <row r="489" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C489" s="7"/>
+    </row>
+    <row r="490" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C490" s="7"/>
+    </row>
+    <row r="491" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C491" s="7"/>
+    </row>
+    <row r="492" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C492" s="7"/>
+    </row>
+    <row r="493" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C493" s="7"/>
+    </row>
+    <row r="494" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C494" s="7"/>
+    </row>
+    <row r="495" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C495" s="7"/>
+    </row>
+    <row r="496" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C496" s="7"/>
+    </row>
+    <row r="497" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C497" s="7"/>
+    </row>
+    <row r="498" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C498" s="7"/>
+    </row>
+    <row r="499" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C499" s="7"/>
+    </row>
+    <row r="500" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C500" s="7"/>
+    </row>
+    <row r="501" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C501" s="7"/>
+    </row>
+    <row r="502" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C502" s="7"/>
+    </row>
+    <row r="503" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C503" s="7"/>
+    </row>
+    <row r="504" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C504" s="7"/>
+    </row>
+    <row r="505" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C505" s="7"/>
+    </row>
+    <row r="506" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C506" s="7"/>
+    </row>
+    <row r="507" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C507" s="7"/>
+    </row>
+    <row r="508" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C508" s="7"/>
+    </row>
+    <row r="509" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C509" s="7"/>
+    </row>
+    <row r="510" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C510" s="7"/>
+    </row>
+    <row r="511" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C511" s="7"/>
+    </row>
+    <row r="512" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C512" s="7"/>
+    </row>
+    <row r="513" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C513" s="7"/>
+    </row>
+    <row r="514" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C514" s="7"/>
+    </row>
+    <row r="515" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C515" s="7"/>
+    </row>
+    <row r="516" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C516" s="7"/>
+    </row>
+    <row r="517" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C517" s="7"/>
+    </row>
+    <row r="518" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C518" s="7"/>
+    </row>
+    <row r="519" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C519" s="7"/>
+    </row>
+    <row r="520" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C520" s="7"/>
+    </row>
+    <row r="521" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C521" s="7"/>
+    </row>
+    <row r="522" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C522" s="7"/>
+    </row>
+    <row r="523" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C523" s="7"/>
+    </row>
+    <row r="524" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C524" s="7"/>
+    </row>
+    <row r="525" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C525" s="7"/>
+    </row>
+    <row r="526" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C526" s="7"/>
+    </row>
+    <row r="527" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C527" s="7"/>
+    </row>
+    <row r="528" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C528" s="7"/>
+    </row>
+    <row r="529" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C529" s="7"/>
+    </row>
+    <row r="530" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C530" s="7"/>
+    </row>
+    <row r="531" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C531" s="7"/>
+    </row>
+    <row r="532" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C532" s="7"/>
+    </row>
+    <row r="533" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C533" s="7"/>
+    </row>
+    <row r="534" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C534" s="7"/>
+    </row>
+    <row r="535" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C535" s="7"/>
+    </row>
+    <row r="536" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C536" s="7"/>
+    </row>
+    <row r="537" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C537" s="7"/>
+    </row>
+    <row r="538" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C538" s="7"/>
+    </row>
+    <row r="539" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C539" s="7"/>
+    </row>
+    <row r="540" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C540" s="7"/>
+    </row>
+    <row r="541" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C541" s="7"/>
+    </row>
+    <row r="542" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C542" s="7"/>
+    </row>
+    <row r="543" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C543" s="7"/>
+    </row>
+    <row r="544" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C544" s="7"/>
+    </row>
+    <row r="545" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C545" s="7"/>
+    </row>
+    <row r="546" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C546" s="7"/>
+    </row>
+    <row r="547" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C547" s="7"/>
+    </row>
+    <row r="548" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C548" s="7"/>
+    </row>
+    <row r="549" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C549" s="7"/>
+    </row>
+    <row r="550" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C550" s="7"/>
+    </row>
+    <row r="551" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C551" s="7"/>
+    </row>
+    <row r="552" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C552" s="7"/>
+    </row>
+    <row r="553" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C553" s="7"/>
+    </row>
+    <row r="554" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C554" s="7"/>
+    </row>
+    <row r="555" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C555" s="7"/>
+    </row>
+    <row r="556" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C556" s="7"/>
+    </row>
+    <row r="557" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C557" s="7"/>
+    </row>
+    <row r="558" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C558" s="7"/>
+    </row>
+    <row r="559" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C559" s="7"/>
+    </row>
+    <row r="560" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C560" s="7"/>
+    </row>
+    <row r="561" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C561" s="7"/>
+    </row>
+    <row r="562" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C562" s="7"/>
+    </row>
+    <row r="563" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C563" s="7"/>
+    </row>
+    <row r="564" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C564" s="7"/>
+    </row>
+    <row r="565" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C565" s="7"/>
+    </row>
+    <row r="566" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C566" s="7"/>
+    </row>
+    <row r="567" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C567" s="7"/>
+    </row>
+    <row r="568" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C568" s="7"/>
+    </row>
+    <row r="569" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C569" s="7"/>
+    </row>
+    <row r="570" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C570" s="7"/>
+    </row>
+    <row r="571" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C571" s="7"/>
+    </row>
+    <row r="572" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C572" s="7"/>
+    </row>
+    <row r="573" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C573" s="7"/>
+    </row>
+    <row r="574" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C574" s="7"/>
+    </row>
+    <row r="575" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C575" s="7"/>
+    </row>
+    <row r="576" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C576" s="7"/>
+    </row>
+    <row r="577" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C577" s="7"/>
+    </row>
+    <row r="578" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C578" s="7"/>
+    </row>
+    <row r="579" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C579" s="7"/>
+    </row>
+    <row r="580" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C580" s="7"/>
+    </row>
+    <row r="581" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C581" s="7"/>
+    </row>
+    <row r="582" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C582" s="7"/>
+    </row>
+    <row r="583" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C583" s="7"/>
+    </row>
+    <row r="584" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C584" s="7"/>
+    </row>
+    <row r="585" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C585" s="7"/>
+    </row>
+    <row r="586" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C586" s="7"/>
+    </row>
+    <row r="587" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C587" s="7"/>
+    </row>
+    <row r="588" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C588" s="7"/>
+    </row>
+    <row r="589" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C589" s="7"/>
+    </row>
+    <row r="590" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C590" s="7"/>
+    </row>
+    <row r="591" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C591" s="7"/>
+    </row>
+    <row r="592" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C592" s="7"/>
+    </row>
+    <row r="593" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C593" s="7"/>
+    </row>
+    <row r="594" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C594" s="7"/>
+    </row>
+    <row r="595" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C595" s="7"/>
+    </row>
+    <row r="596" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C596" s="7"/>
+    </row>
+    <row r="597" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C597" s="7"/>
+    </row>
+    <row r="598" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C598" s="7"/>
+    </row>
+    <row r="599" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C599" s="7"/>
+    </row>
+    <row r="600" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C600" s="7"/>
+    </row>
+    <row r="601" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C601" s="7"/>
+    </row>
+    <row r="602" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C602" s="7"/>
+    </row>
+    <row r="603" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C603" s="7"/>
+    </row>
+    <row r="604" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C604" s="7"/>
+    </row>
+    <row r="605" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C605" s="7"/>
+    </row>
+    <row r="606" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C606" s="7"/>
+    </row>
+    <row r="607" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C607" s="7"/>
+    </row>
+    <row r="608" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C608" s="7"/>
+    </row>
+    <row r="609" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C609" s="7"/>
+    </row>
+    <row r="610" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C610" s="7"/>
+    </row>
+    <row r="611" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C611" s="7"/>
+    </row>
+    <row r="612" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C612" s="7"/>
+    </row>
+    <row r="613" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C613" s="7"/>
+    </row>
+    <row r="614" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C614" s="7"/>
+    </row>
+    <row r="615" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C615" s="7"/>
+    </row>
+    <row r="616" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C616" s="7"/>
+    </row>
+    <row r="617" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C617" s="7"/>
+    </row>
+    <row r="618" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C618" s="7"/>
+    </row>
+    <row r="619" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C619" s="7"/>
+    </row>
+    <row r="620" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C620" s="7"/>
+    </row>
+    <row r="621" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C621" s="7"/>
+    </row>
+    <row r="622" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C622" s="7"/>
+    </row>
+    <row r="623" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C623" s="7"/>
+    </row>
+    <row r="624" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C624" s="7"/>
+    </row>
+    <row r="625" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C625" s="7"/>
+    </row>
+    <row r="626" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C626" s="7"/>
+    </row>
+    <row r="627" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C627" s="7"/>
+    </row>
+    <row r="628" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C628" s="7"/>
+    </row>
+    <row r="629" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C629" s="7"/>
+    </row>
+    <row r="630" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C630" s="7"/>
+    </row>
+    <row r="631" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C631" s="7"/>
+    </row>
+    <row r="632" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C632" s="7"/>
+    </row>
+    <row r="633" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C633" s="7"/>
+    </row>
+    <row r="634" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C634" s="7"/>
+    </row>
+    <row r="635" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C635" s="7"/>
+    </row>
+    <row r="636" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C636" s="7"/>
+    </row>
+    <row r="637" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C637" s="7"/>
+    </row>
+    <row r="638" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C638" s="7"/>
+    </row>
+    <row r="639" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C639" s="7"/>
+    </row>
+    <row r="640" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C640" s="7"/>
+    </row>
+    <row r="641" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C641" s="7"/>
+    </row>
+    <row r="642" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C642" s="7"/>
+    </row>
+    <row r="643" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C643" s="7"/>
+    </row>
+    <row r="644" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C644" s="7"/>
+    </row>
+    <row r="645" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C645" s="7"/>
+    </row>
+    <row r="646" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C646" s="7"/>
+    </row>
+    <row r="647" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C647" s="7"/>
+    </row>
+    <row r="648" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C648" s="7"/>
+    </row>
+    <row r="649" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C649" s="7"/>
+    </row>
+    <row r="650" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C650" s="7"/>
+    </row>
+    <row r="651" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C651" s="7"/>
+    </row>
+    <row r="652" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C652" s="7"/>
+    </row>
+    <row r="653" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C653" s="7"/>
+    </row>
+    <row r="654" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C654" s="7"/>
+    </row>
+    <row r="655" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C655" s="7"/>
+    </row>
+    <row r="656" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C656" s="7"/>
+    </row>
+    <row r="657" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C657" s="7"/>
+    </row>
+    <row r="658" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C658" s="7"/>
+    </row>
+    <row r="659" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C659" s="7"/>
+    </row>
+    <row r="660" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C660" s="7"/>
+    </row>
+    <row r="661" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C661" s="7"/>
+    </row>
+    <row r="662" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C662" s="7"/>
+    </row>
+    <row r="663" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C663" s="7"/>
+    </row>
+    <row r="664" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C664" s="7"/>
+    </row>
+    <row r="665" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C665" s="7"/>
+    </row>
+    <row r="666" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C666" s="7"/>
+    </row>
+    <row r="667" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C667" s="7"/>
+    </row>
+    <row r="668" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C668" s="7"/>
+    </row>
+    <row r="669" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C669" s="7"/>
+    </row>
+    <row r="670" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C670" s="7"/>
+    </row>
+    <row r="671" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C671" s="7"/>
+    </row>
+    <row r="672" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C672" s="7"/>
+    </row>
+    <row r="673" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C673" s="7"/>
+    </row>
+    <row r="674" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C674" s="7"/>
+    </row>
+    <row r="675" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C675" s="7"/>
+    </row>
+    <row r="676" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C676" s="7"/>
+    </row>
+    <row r="677" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C677" s="7"/>
+    </row>
+    <row r="678" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C678" s="7"/>
+    </row>
+    <row r="679" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C679" s="7"/>
+    </row>
+    <row r="680" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C680" s="7"/>
+    </row>
+    <row r="681" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C681" s="7"/>
+    </row>
+    <row r="682" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C682" s="7"/>
+    </row>
+    <row r="683" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C683" s="7"/>
+    </row>
+    <row r="684" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C684" s="7"/>
+    </row>
+    <row r="685" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C685" s="7"/>
+    </row>
+    <row r="686" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C686" s="7"/>
+    </row>
+    <row r="687" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C687" s="7"/>
+    </row>
+    <row r="688" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C688" s="7"/>
+    </row>
+    <row r="689" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C689" s="7"/>
+    </row>
+    <row r="690" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C690" s="7"/>
+    </row>
+    <row r="691" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C691" s="7"/>
+    </row>
+    <row r="692" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C692" s="7"/>
+    </row>
+    <row r="693" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C693" s="7"/>
+    </row>
+    <row r="694" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C694" s="7"/>
+    </row>
+    <row r="695" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C695" s="7"/>
+    </row>
+    <row r="696" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C696" s="7"/>
+    </row>
+    <row r="697" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C697" s="7"/>
+    </row>
+    <row r="698" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C698" s="7"/>
+    </row>
+    <row r="699" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C699" s="7"/>
+    </row>
+    <row r="700" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C700" s="7"/>
+    </row>
+    <row r="701" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C701" s="7"/>
+    </row>
+    <row r="702" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C702" s="7"/>
+    </row>
+    <row r="703" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C703" s="7"/>
+    </row>
+    <row r="704" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C704" s="7"/>
+    </row>
+    <row r="705" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C705" s="7"/>
+    </row>
+    <row r="706" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C706" s="7"/>
+    </row>
+    <row r="707" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C707" s="7"/>
+    </row>
+    <row r="708" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C708" s="7"/>
+    </row>
+    <row r="709" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C709" s="7"/>
+    </row>
+    <row r="710" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C710" s="7"/>
+    </row>
+    <row r="711" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C711" s="7"/>
+    </row>
+    <row r="712" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C712" s="7"/>
+    </row>
+    <row r="713" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C713" s="7"/>
+    </row>
+    <row r="714" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C714" s="7"/>
+    </row>
+    <row r="715" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C715" s="7"/>
+    </row>
+    <row r="716" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C716" s="7"/>
+    </row>
+    <row r="717" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C717" s="7"/>
+    </row>
+    <row r="718" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C718" s="7"/>
+    </row>
+    <row r="719" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C719" s="7"/>
+    </row>
+    <row r="720" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C720" s="7"/>
+    </row>
+    <row r="721" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C721" s="7"/>
+    </row>
+    <row r="722" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C722" s="7"/>
+    </row>
+    <row r="723" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C723" s="7"/>
+    </row>
+    <row r="724" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C724" s="7"/>
+    </row>
+    <row r="725" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C725" s="7"/>
+    </row>
+    <row r="726" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C726" s="7"/>
+    </row>
+    <row r="727" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C727" s="7"/>
+    </row>
+    <row r="728" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C728" s="7"/>
+    </row>
+    <row r="729" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C729" s="7"/>
+    </row>
+    <row r="730" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C730" s="7"/>
+    </row>
+    <row r="731" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C731" s="7"/>
+    </row>
+    <row r="732" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C732" s="7"/>
+    </row>
+    <row r="733" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C733" s="7"/>
+    </row>
+    <row r="734" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C734" s="7"/>
+    </row>
+    <row r="735" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C735" s="7"/>
+    </row>
+    <row r="736" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C736" s="7"/>
+    </row>
+    <row r="737" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C737" s="7"/>
+    </row>
+    <row r="738" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C738" s="7"/>
+    </row>
+    <row r="739" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C739" s="7"/>
+    </row>
+    <row r="740" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C740" s="7"/>
+    </row>
+    <row r="741" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C741" s="7"/>
+    </row>
+    <row r="742" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C742" s="7"/>
+    </row>
+    <row r="743" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C743" s="7"/>
+    </row>
+    <row r="744" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C744" s="7"/>
+    </row>
+    <row r="745" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C745" s="7"/>
+    </row>
+    <row r="746" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C746" s="7"/>
+    </row>
+    <row r="747" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C747" s="7"/>
+    </row>
+    <row r="748" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C748" s="7"/>
+    </row>
+    <row r="749" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C749" s="7"/>
+    </row>
+    <row r="750" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C750" s="7"/>
+    </row>
+    <row r="751" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C751" s="7"/>
+    </row>
+    <row r="752" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C752" s="7"/>
+    </row>
+    <row r="753" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C753" s="7"/>
+    </row>
+    <row r="754" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C754" s="7"/>
+    </row>
+    <row r="755" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C755" s="7"/>
+    </row>
+    <row r="756" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C756" s="7"/>
+    </row>
+    <row r="757" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C757" s="7"/>
+    </row>
+    <row r="758" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C758" s="7"/>
+    </row>
+    <row r="759" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C759" s="7"/>
+    </row>
+    <row r="760" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C760" s="7"/>
+    </row>
+    <row r="761" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C761" s="7"/>
+    </row>
+    <row r="762" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C762" s="7"/>
+    </row>
+    <row r="763" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C763" s="7"/>
+    </row>
+    <row r="764" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C764" s="7"/>
+    </row>
+    <row r="765" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C765" s="7"/>
+    </row>
+    <row r="766" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C766" s="7"/>
+    </row>
+    <row r="767" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C767" s="7"/>
+    </row>
+    <row r="768" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C768" s="7"/>
+    </row>
+    <row r="769" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C769" s="7"/>
+    </row>
+    <row r="770" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C770" s="7"/>
+    </row>
+    <row r="771" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C771" s="7"/>
+    </row>
+    <row r="772" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C772" s="7"/>
+    </row>
+    <row r="773" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C773" s="7"/>
+    </row>
+    <row r="774" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C774" s="7"/>
+    </row>
+    <row r="775" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C775" s="7"/>
+    </row>
+    <row r="776" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C776" s="7"/>
+    </row>
+    <row r="777" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C777" s="7"/>
+    </row>
+    <row r="778" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C778" s="7"/>
+    </row>
+    <row r="779" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C779" s="7"/>
+    </row>
+    <row r="780" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C780" s="7"/>
+    </row>
+    <row r="781" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C781" s="7"/>
+    </row>
+    <row r="782" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C782" s="7"/>
+    </row>
+    <row r="783" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C783" s="7"/>
+    </row>
+    <row r="784" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C784" s="7"/>
+    </row>
+    <row r="785" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C785" s="7"/>
+    </row>
+    <row r="786" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C786" s="7"/>
+    </row>
+    <row r="787" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C787" s="7"/>
+    </row>
+    <row r="788" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C788" s="7"/>
+    </row>
+    <row r="789" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C789" s="7"/>
+    </row>
+    <row r="790" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C790" s="7"/>
+    </row>
+    <row r="791" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C791" s="7"/>
+    </row>
+    <row r="792" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C792" s="7"/>
+    </row>
+    <row r="793" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C793" s="7"/>
+    </row>
+    <row r="794" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C794" s="7"/>
+    </row>
+    <row r="795" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C795" s="7"/>
+    </row>
+    <row r="796" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C796" s="7"/>
+    </row>
+    <row r="797" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C797" s="7"/>
+    </row>
+    <row r="798" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C798" s="7"/>
+    </row>
+    <row r="799" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C799" s="7"/>
+    </row>
+    <row r="800" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C800" s="7"/>
+    </row>
+    <row r="801" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C801" s="7"/>
+    </row>
+    <row r="802" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C802" s="7"/>
+    </row>
+    <row r="803" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C803" s="7"/>
+    </row>
+    <row r="804" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C804" s="7"/>
+    </row>
+    <row r="805" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C805" s="7"/>
+    </row>
+    <row r="806" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C806" s="7"/>
+    </row>
+    <row r="807" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C807" s="7"/>
+    </row>
+    <row r="808" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C808" s="7"/>
+    </row>
+    <row r="809" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C809" s="7"/>
+    </row>
+    <row r="810" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C810" s="7"/>
+    </row>
+    <row r="811" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C811" s="7"/>
+    </row>
+    <row r="812" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C812" s="7"/>
+    </row>
+    <row r="813" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C813" s="7"/>
+    </row>
+    <row r="814" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C814" s="7"/>
+    </row>
+    <row r="815" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C815" s="7"/>
+    </row>
+    <row r="816" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C816" s="7"/>
+    </row>
+    <row r="817" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C817" s="7"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0.6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>